<commit_message>
Drew debris sprites for Player Ship & Small Goblin Ship
Also added a new sheet to EnemyDirector.xlsx
</commit_message>
<xml_diff>
--- a/EnemyDirector.xlsx
+++ b/EnemyDirector.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cameron\Desktop\Files\ProjectileGameProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\PROJECTS\ProjectileGameProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC337FA1-BD2A-4995-8989-D1BB8AB0187D}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A693723-1232-4EB3-A43B-67FCA61E7F1B}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="5240" activeTab="1" xr2:uid="{CBD09E6E-C96C-4EBB-B85B-FCB6E107760C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14385" windowHeight="5235" activeTab="2" xr2:uid="{CBD09E6E-C96C-4EBB-B85B-FCB6E107760C}"/>
   </bookViews>
   <sheets>
-    <sheet name="current" sheetId="1" r:id="rId1"/>
-    <sheet name="future" sheetId="2" r:id="rId2"/>
+    <sheet name="Version 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Version 2" sheetId="2" r:id="rId2"/>
+    <sheet name="Version 2 - Full Dynamic X" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="67">
   <si>
     <t>LVL 1</t>
   </si>
@@ -192,6 +193,42 @@
   <si>
     <t>IF(X%2)==0, OUTPUT = (X+3)/3</t>
   </si>
+  <si>
+    <t>Enemy</t>
+  </si>
+  <si>
+    <t>Grey Asteroid LV1</t>
+  </si>
+  <si>
+    <t>Grey Asteroid LV2</t>
+  </si>
+  <si>
+    <t>Grey Asteroid LV3</t>
+  </si>
+  <si>
+    <t>White Asteroid LV1</t>
+  </si>
+  <si>
+    <t>White Asteroid LV2</t>
+  </si>
+  <si>
+    <t>White Asteroid LV3</t>
+  </si>
+  <si>
+    <t>Goblin Fighter Large</t>
+  </si>
+  <si>
+    <t>Goblin Fighter Small</t>
+  </si>
+  <si>
+    <t>Total Enemies Spawned</t>
+  </si>
+  <si>
+    <t>Total Enemies Generated</t>
+  </si>
+  <si>
+    <t>Total Persistend Enemies</t>
+  </si>
 </sst>
 </file>
 
@@ -206,7 +243,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -234,6 +271,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -580,7 +623,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
@@ -646,6 +689,24 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -755,7 +816,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>future!$M$1:$AA$1</c:f>
+              <c:f>'Version 2'!$M$1:$AA$1</c:f>
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
@@ -808,7 +869,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>future!$M$14:$AA$14</c:f>
+              <c:f>'Version 2'!$M$14:$AA$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -1136,7 +1197,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>future!$M$1:$AA$1</c:f>
+              <c:f>'Version 2'!$M$1:$AA$1</c:f>
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
@@ -1189,7 +1250,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>future!$M$15:$AA$15</c:f>
+              <c:f>'Version 2'!$M$15:$AA$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -1425,6 +1486,958 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="20" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-NZ" baseline="0"/>
+              <a:t>Total Enemies per Level</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="20" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="5.0303631665661819E-2"/>
+          <c:y val="0.10082227939006162"/>
+          <c:w val="0.93046785500272755"/>
+          <c:h val="0.78179191710297036"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Enemies Spawned by Director</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Version 2 - Full Dynamic X'!$C$1:$V$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Version 2 - Full Dynamic X'!$C$10:$V$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>39</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B513-4DE1-BED3-57056EAF5593}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Enemies Spawned Total</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>'Version 2 - Full Dynamic X'!$C$12:$V$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>107</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>119</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>122</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>124</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>137</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>149</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-B513-4DE1-BED3-57056EAF5593}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="t"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:dropLines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="35000"/>
+                  <a:lumOff val="65000"/>
+                  <a:alpha val="33000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:dropLines>
+        <c:smooth val="0"/>
+        <c:axId val="592277000"/>
+        <c:axId val="592279296"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="2"/>
+                <c:order val="2"/>
+                <c:tx>
+                  <c:v>Persistent Enemies</c:v>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="22225" cap="rnd" cmpd="sng" algn="ctr">
+                    <a:solidFill>
+                      <a:schemeClr val="accent6"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
+                <c:dLbls>
+                  <c:spPr>
+                    <a:noFill/>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                  <c:txPr>
+                    <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                      <a:spAutoFit/>
+                    </a:bodyPr>
+                    <a:lstStyle/>
+                    <a:p>
+                      <a:pPr>
+                        <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                          <a:solidFill>
+                            <a:schemeClr val="dk1">
+                              <a:lumMod val="65000"/>
+                              <a:lumOff val="35000"/>
+                            </a:schemeClr>
+                          </a:solidFill>
+                          <a:latin typeface="+mn-lt"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:defRPr>
+                      </a:pPr>
+                      <a:endParaRPr lang="en-US"/>
+                    </a:p>
+                  </c:txPr>
+                  <c:dLblPos val="t"/>
+                  <c:showLegendKey val="0"/>
+                  <c:showVal val="1"/>
+                  <c:showCatName val="0"/>
+                  <c:showSerName val="0"/>
+                  <c:showPercent val="0"/>
+                  <c:showBubbleSize val="0"/>
+                  <c:showLeaderLines val="0"/>
+                  <c:extLst>
+                    <c:ext uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                      <c15:showLeaderLines val="1"/>
+                      <c15:leaderLines>
+                        <c:spPr>
+                          <a:ln w="9525">
+                            <a:solidFill>
+                              <a:schemeClr val="dk1">
+                                <a:lumMod val="35000"/>
+                                <a:lumOff val="65000"/>
+                              </a:schemeClr>
+                            </a:solidFill>
+                          </a:ln>
+                          <a:effectLst/>
+                        </c:spPr>
+                      </c15:leaderLines>
+                    </c:ext>
+                  </c:extLst>
+                </c:dLbls>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Version 2 - Full Dynamic X'!$C$11:$V$11</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="20"/>
+                      <c:pt idx="0">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>18</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>16</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>32</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>30</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>37</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>33</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>48</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>46</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>52</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>47</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>65</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>59</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>67</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>64</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>80</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000004-B513-4DE1-BED3-57056EAF5593}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+          </c:ext>
+        </c:extLst>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="592277000"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-NZ"/>
+                  <a:t>Level</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-NZ" baseline="0"/>
+                  <a:t> X</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="20" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="592279296"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="592279296"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-NZ"/>
+                  <a:t># of Enemies</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="20" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="592277000"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="lt1"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.1101621396691123"/>
+          <c:y val="0.16882744119076723"/>
+          <c:w val="0.13532118674034216"/>
+          <c:h val="8.7125462226688669E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1505,6 +2518,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="230">
   <cs:axisTitle>
@@ -2044,6 +3097,544 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="230">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" b="0" kern="1200" spc="20" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="2">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="1"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:shade val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="2">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="1"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:shade val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="4"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+            <a:alpha val="33000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill>
+        <a:gsLst>
+          <a:gs pos="100000">
+            <a:schemeClr val="lt1">
+              <a:lumMod val="95000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="0">
+            <a:schemeClr val="lt1"/>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+    </cs:spPr>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" kern="1200" cap="none" spc="20" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" spc="20" baseline="0"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="230">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2650,6 +4241,47 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1247774</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>61911</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C9F26A1A-24B2-40DA-A82E-84B112BAA193}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2961,9 +4593,9 @@
       <selection activeCell="K9" sqref="A1:K9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="10"/>
       <c r="B1" s="29" t="s">
         <v>0</v>
@@ -2996,7 +4628,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
         <v>10</v>
       </c>
@@ -3019,7 +4651,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>11</v>
       </c>
@@ -3048,7 +4680,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>12</v>
       </c>
@@ -3075,7 +4707,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>13</v>
       </c>
@@ -3098,7 +4730,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>14</v>
       </c>
@@ -3121,7 +4753,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
         <v>15</v>
       </c>
@@ -3146,7 +4778,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
         <v>16</v>
       </c>
@@ -3173,7 +4805,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
         <v>17</v>
       </c>
@@ -3205,17 +4837,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1042877E-8AE6-4508-9AFE-80CA993047BE}">
   <dimension ref="A1:AA19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.1796875" customWidth="1"/>
-    <col min="12" max="12" width="30.1796875" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" customWidth="1"/>
+    <col min="12" max="12" width="30.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" s="10"/>
       <c r="B1" s="29" t="s">
         <v>0</v>
@@ -3296,7 +4928,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
         <v>10</v>
       </c>
@@ -3369,7 +5001,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>11</v>
       </c>
@@ -3448,7 +5080,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>12</v>
       </c>
@@ -3525,7 +5157,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>13</v>
       </c>
@@ -3602,7 +5234,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>14</v>
       </c>
@@ -3675,7 +5307,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
         <v>15</v>
       </c>
@@ -3750,7 +5382,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
         <v>16</v>
       </c>
@@ -3821,7 +5453,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
         <v>17</v>
       </c>
@@ -3888,7 +5520,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" s="37" t="s">
         <v>18</v>
       </c>
@@ -3993,7 +5625,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" s="37" t="s">
         <v>52</v>
       </c>
@@ -4099,7 +5731,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" s="37" t="s">
         <v>20</v>
       </c>
@@ -4116,7 +5748,7 @@
       <c r="J16" s="47"/>
       <c r="K16" s="48"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>43</v>
       </c>
@@ -4139,7 +5771,7 @@
       </c>
       <c r="K17" s="3"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B18" s="4" t="s">
         <v>48</v>
       </c>
@@ -4155,7 +5787,7 @@
       <c r="J18" s="5"/>
       <c r="K18" s="6"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B19" s="7" t="s">
         <v>49</v>
       </c>
@@ -4173,4 +5805,1051 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A18C6132-7A51-448D-9D07-9F2552FED37B}">
+  <dimension ref="A1:V12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="X9" sqref="X9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A1" s="52" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="52" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="53">
+        <v>1</v>
+      </c>
+      <c r="D1" s="53">
+        <v>2</v>
+      </c>
+      <c r="E1" s="54">
+        <v>3</v>
+      </c>
+      <c r="F1" s="53">
+        <v>4</v>
+      </c>
+      <c r="G1" s="53">
+        <v>5</v>
+      </c>
+      <c r="H1" s="54">
+        <v>6</v>
+      </c>
+      <c r="I1" s="53">
+        <v>7</v>
+      </c>
+      <c r="J1" s="53">
+        <v>8</v>
+      </c>
+      <c r="K1" s="54">
+        <v>9</v>
+      </c>
+      <c r="L1" s="53">
+        <v>10</v>
+      </c>
+      <c r="M1" s="53">
+        <v>11</v>
+      </c>
+      <c r="N1" s="54">
+        <v>12</v>
+      </c>
+      <c r="O1" s="53">
+        <v>13</v>
+      </c>
+      <c r="P1" s="53">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="55">
+        <v>15</v>
+      </c>
+      <c r="R1" s="55">
+        <v>16</v>
+      </c>
+      <c r="S1" s="55">
+        <v>17</v>
+      </c>
+      <c r="T1" s="55">
+        <v>18</v>
+      </c>
+      <c r="U1" s="55">
+        <v>19</v>
+      </c>
+      <c r="V1" s="55">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A2" s="49" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="49" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="11">
+        <f>IF(MOD(C1,2)=1,QUOTIENT(C1+3,3),0)</f>
+        <v>1</v>
+      </c>
+      <c r="D2" s="11">
+        <f t="shared" ref="D2:H2" si="0">IF(MOD(D1,2)=1,QUOTIENT(D1+3,3),0)</f>
+        <v>0</v>
+      </c>
+      <c r="E2" s="11">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="F2" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G2" s="11">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="H2" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I2" s="11">
+        <f t="shared" ref="I2" si="1">IF(MOD(I1,2)=1,QUOTIENT(I1+3,3),0)</f>
+        <v>3</v>
+      </c>
+      <c r="J2" s="11">
+        <f t="shared" ref="J2" si="2">IF(MOD(J1,2)=1,QUOTIENT(J1+3,3),0)</f>
+        <v>0</v>
+      </c>
+      <c r="K2" s="11">
+        <f t="shared" ref="K2" si="3">IF(MOD(K1,2)=1,QUOTIENT(K1+3,3),0)</f>
+        <v>4</v>
+      </c>
+      <c r="L2" s="11">
+        <f t="shared" ref="L2:M2" si="4">IF(MOD(L1,2)=1,QUOTIENT(L1+3,3),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M2" s="11">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="N2" s="11">
+        <f t="shared" ref="N2" si="5">IF(MOD(N1,2)=1,QUOTIENT(N1+3,3),0)</f>
+        <v>0</v>
+      </c>
+      <c r="O2" s="11">
+        <f t="shared" ref="O2" si="6">IF(MOD(O1,2)=1,QUOTIENT(O1+3,3),0)</f>
+        <v>5</v>
+      </c>
+      <c r="P2" s="11">
+        <f t="shared" ref="P2" si="7">IF(MOD(P1,2)=1,QUOTIENT(P1+3,3),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q2" s="41">
+        <f t="shared" ref="Q2" si="8">IF(MOD(Q1,2)=1,QUOTIENT(Q1+3,3),0)</f>
+        <v>6</v>
+      </c>
+      <c r="R2" s="41">
+        <f t="shared" ref="R2" si="9">IF(MOD(R1,2)=1,QUOTIENT(R1+3,3),0)</f>
+        <v>0</v>
+      </c>
+      <c r="S2" s="41">
+        <f t="shared" ref="S2" si="10">IF(MOD(S1,2)=1,QUOTIENT(S1+3,3),0)</f>
+        <v>6</v>
+      </c>
+      <c r="T2" s="41">
+        <f t="shared" ref="T2" si="11">IF(MOD(T1,2)=1,QUOTIENT(T1+3,3),0)</f>
+        <v>0</v>
+      </c>
+      <c r="U2" s="41">
+        <f t="shared" ref="U2" si="12">IF(MOD(U1,2)=1,QUOTIENT(U1+3,3),0)</f>
+        <v>7</v>
+      </c>
+      <c r="V2" s="41">
+        <f t="shared" ref="V2" si="13">IF(MOD(V1,2)=1,QUOTIENT(V1+3,3),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A3" s="45" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" s="45" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="13">
+        <f>QUOTIENT(C1+4,3)</f>
+        <v>1</v>
+      </c>
+      <c r="D3" s="13">
+        <f t="shared" ref="D3:Q3" si="14">QUOTIENT(D1+4,3)</f>
+        <v>2</v>
+      </c>
+      <c r="E3" s="13">
+        <f t="shared" si="14"/>
+        <v>2</v>
+      </c>
+      <c r="F3" s="13">
+        <f t="shared" si="14"/>
+        <v>2</v>
+      </c>
+      <c r="G3" s="13">
+        <f t="shared" si="14"/>
+        <v>3</v>
+      </c>
+      <c r="H3" s="13">
+        <f t="shared" si="14"/>
+        <v>3</v>
+      </c>
+      <c r="I3" s="13">
+        <f t="shared" si="14"/>
+        <v>3</v>
+      </c>
+      <c r="J3" s="13">
+        <f t="shared" si="14"/>
+        <v>4</v>
+      </c>
+      <c r="K3" s="13">
+        <f t="shared" si="14"/>
+        <v>4</v>
+      </c>
+      <c r="L3" s="13">
+        <f t="shared" si="14"/>
+        <v>4</v>
+      </c>
+      <c r="M3" s="13">
+        <f t="shared" si="14"/>
+        <v>5</v>
+      </c>
+      <c r="N3" s="13">
+        <f t="shared" si="14"/>
+        <v>5</v>
+      </c>
+      <c r="O3" s="13">
+        <f t="shared" si="14"/>
+        <v>5</v>
+      </c>
+      <c r="P3" s="13">
+        <f t="shared" si="14"/>
+        <v>6</v>
+      </c>
+      <c r="Q3" s="42">
+        <f t="shared" si="14"/>
+        <v>6</v>
+      </c>
+      <c r="R3" s="42">
+        <f t="shared" ref="R3:V3" si="15">QUOTIENT(R1+4,3)</f>
+        <v>6</v>
+      </c>
+      <c r="S3" s="42">
+        <f t="shared" si="15"/>
+        <v>7</v>
+      </c>
+      <c r="T3" s="42">
+        <f t="shared" si="15"/>
+        <v>7</v>
+      </c>
+      <c r="U3" s="42">
+        <f t="shared" si="15"/>
+        <v>7</v>
+      </c>
+      <c r="V3" s="42">
+        <f t="shared" si="15"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A4" s="46" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4" s="46" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="15">
+        <f>QUOTIENT(C1+1,4)</f>
+        <v>0</v>
+      </c>
+      <c r="D4" s="15">
+        <f t="shared" ref="D4:Q4" si="16">QUOTIENT(D1+1,4)</f>
+        <v>0</v>
+      </c>
+      <c r="E4" s="15">
+        <f t="shared" si="16"/>
+        <v>1</v>
+      </c>
+      <c r="F4" s="15">
+        <f t="shared" si="16"/>
+        <v>1</v>
+      </c>
+      <c r="G4" s="15">
+        <f t="shared" si="16"/>
+        <v>1</v>
+      </c>
+      <c r="H4" s="15">
+        <f t="shared" si="16"/>
+        <v>1</v>
+      </c>
+      <c r="I4" s="15">
+        <f t="shared" si="16"/>
+        <v>2</v>
+      </c>
+      <c r="J4" s="15">
+        <f t="shared" si="16"/>
+        <v>2</v>
+      </c>
+      <c r="K4" s="15">
+        <f t="shared" si="16"/>
+        <v>2</v>
+      </c>
+      <c r="L4" s="15">
+        <f t="shared" si="16"/>
+        <v>2</v>
+      </c>
+      <c r="M4" s="15">
+        <f t="shared" si="16"/>
+        <v>3</v>
+      </c>
+      <c r="N4" s="15">
+        <f t="shared" si="16"/>
+        <v>3</v>
+      </c>
+      <c r="O4" s="15">
+        <f t="shared" si="16"/>
+        <v>3</v>
+      </c>
+      <c r="P4" s="15">
+        <f t="shared" si="16"/>
+        <v>3</v>
+      </c>
+      <c r="Q4" s="43">
+        <f t="shared" si="16"/>
+        <v>4</v>
+      </c>
+      <c r="R4" s="43">
+        <f t="shared" ref="R4:V4" si="17">QUOTIENT(R1+1,4)</f>
+        <v>4</v>
+      </c>
+      <c r="S4" s="43">
+        <f t="shared" si="17"/>
+        <v>4</v>
+      </c>
+      <c r="T4" s="43">
+        <f t="shared" si="17"/>
+        <v>4</v>
+      </c>
+      <c r="U4" s="43">
+        <f t="shared" si="17"/>
+        <v>5</v>
+      </c>
+      <c r="V4" s="43">
+        <f t="shared" si="17"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A5" s="45" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" s="45" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" s="11">
+        <f>IF(MOD(C1,2)=0,QUOTIENT(C1+3,3),0)</f>
+        <v>0</v>
+      </c>
+      <c r="D5" s="11">
+        <f t="shared" ref="D5:Q5" si="18">IF(MOD(D1,2)=0,QUOTIENT(D1+3,3),0)</f>
+        <v>1</v>
+      </c>
+      <c r="E5" s="11">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="F5" s="11">
+        <f t="shared" si="18"/>
+        <v>2</v>
+      </c>
+      <c r="G5" s="11">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="H5" s="11">
+        <f t="shared" si="18"/>
+        <v>3</v>
+      </c>
+      <c r="I5" s="11">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="J5" s="11">
+        <f t="shared" si="18"/>
+        <v>3</v>
+      </c>
+      <c r="K5" s="11">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="L5" s="11">
+        <f t="shared" si="18"/>
+        <v>4</v>
+      </c>
+      <c r="M5" s="11">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="N5" s="11">
+        <f t="shared" si="18"/>
+        <v>5</v>
+      </c>
+      <c r="O5" s="11">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="P5" s="11">
+        <f t="shared" si="18"/>
+        <v>5</v>
+      </c>
+      <c r="Q5" s="41">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="R5" s="41">
+        <f t="shared" ref="R5:V5" si="19">IF(MOD(R1,2)=0,QUOTIENT(R1+3,3),0)</f>
+        <v>6</v>
+      </c>
+      <c r="S5" s="41">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="T5" s="41">
+        <f t="shared" si="19"/>
+        <v>7</v>
+      </c>
+      <c r="U5" s="41">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="V5" s="41">
+        <f t="shared" si="19"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A6" s="45" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6" s="45" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="13">
+        <f>QUOTIENT(C1+2,3)</f>
+        <v>1</v>
+      </c>
+      <c r="D6" s="13">
+        <f t="shared" ref="D6:Q6" si="20">QUOTIENT(D1+2,3)</f>
+        <v>1</v>
+      </c>
+      <c r="E6" s="13">
+        <f t="shared" si="20"/>
+        <v>1</v>
+      </c>
+      <c r="F6" s="13">
+        <f t="shared" si="20"/>
+        <v>2</v>
+      </c>
+      <c r="G6" s="13">
+        <f t="shared" si="20"/>
+        <v>2</v>
+      </c>
+      <c r="H6" s="13">
+        <f t="shared" si="20"/>
+        <v>2</v>
+      </c>
+      <c r="I6" s="13">
+        <f t="shared" si="20"/>
+        <v>3</v>
+      </c>
+      <c r="J6" s="13">
+        <f t="shared" si="20"/>
+        <v>3</v>
+      </c>
+      <c r="K6" s="13">
+        <f t="shared" si="20"/>
+        <v>3</v>
+      </c>
+      <c r="L6" s="13">
+        <f t="shared" si="20"/>
+        <v>4</v>
+      </c>
+      <c r="M6" s="13">
+        <f t="shared" si="20"/>
+        <v>4</v>
+      </c>
+      <c r="N6" s="13">
+        <f t="shared" si="20"/>
+        <v>4</v>
+      </c>
+      <c r="O6" s="13">
+        <f t="shared" si="20"/>
+        <v>5</v>
+      </c>
+      <c r="P6" s="13">
+        <f t="shared" si="20"/>
+        <v>5</v>
+      </c>
+      <c r="Q6" s="42">
+        <f t="shared" si="20"/>
+        <v>5</v>
+      </c>
+      <c r="R6" s="42">
+        <f t="shared" ref="R6:V6" si="21">QUOTIENT(R1+2,3)</f>
+        <v>6</v>
+      </c>
+      <c r="S6" s="42">
+        <f t="shared" si="21"/>
+        <v>6</v>
+      </c>
+      <c r="T6" s="42">
+        <f t="shared" si="21"/>
+        <v>6</v>
+      </c>
+      <c r="U6" s="42">
+        <f t="shared" si="21"/>
+        <v>7</v>
+      </c>
+      <c r="V6" s="42">
+        <f t="shared" si="21"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A7" s="45" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7" s="45" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="15">
+        <f>QUOTIENT(C1,4)</f>
+        <v>0</v>
+      </c>
+      <c r="D7" s="15">
+        <f t="shared" ref="D7:Q7" si="22">QUOTIENT(D1,4)</f>
+        <v>0</v>
+      </c>
+      <c r="E7" s="15">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="F7" s="15">
+        <f t="shared" si="22"/>
+        <v>1</v>
+      </c>
+      <c r="G7" s="15">
+        <f t="shared" si="22"/>
+        <v>1</v>
+      </c>
+      <c r="H7" s="15">
+        <f t="shared" si="22"/>
+        <v>1</v>
+      </c>
+      <c r="I7" s="15">
+        <f t="shared" si="22"/>
+        <v>1</v>
+      </c>
+      <c r="J7" s="15">
+        <f t="shared" si="22"/>
+        <v>2</v>
+      </c>
+      <c r="K7" s="15">
+        <f t="shared" si="22"/>
+        <v>2</v>
+      </c>
+      <c r="L7" s="15">
+        <f t="shared" si="22"/>
+        <v>2</v>
+      </c>
+      <c r="M7" s="15">
+        <f t="shared" si="22"/>
+        <v>2</v>
+      </c>
+      <c r="N7" s="15">
+        <f t="shared" si="22"/>
+        <v>3</v>
+      </c>
+      <c r="O7" s="15">
+        <f t="shared" si="22"/>
+        <v>3</v>
+      </c>
+      <c r="P7" s="15">
+        <f t="shared" si="22"/>
+        <v>3</v>
+      </c>
+      <c r="Q7" s="43">
+        <f t="shared" si="22"/>
+        <v>3</v>
+      </c>
+      <c r="R7" s="43">
+        <f t="shared" ref="R7:V7" si="23">QUOTIENT(R1,4)</f>
+        <v>4</v>
+      </c>
+      <c r="S7" s="43">
+        <f t="shared" si="23"/>
+        <v>4</v>
+      </c>
+      <c r="T7" s="43">
+        <f t="shared" si="23"/>
+        <v>4</v>
+      </c>
+      <c r="U7" s="43">
+        <f t="shared" si="23"/>
+        <v>4</v>
+      </c>
+      <c r="V7" s="43">
+        <f t="shared" si="23"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A8" s="49" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8" s="49" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="13">
+        <f>QUOTIENT(C1+1,5)</f>
+        <v>0</v>
+      </c>
+      <c r="D8" s="13">
+        <f t="shared" ref="D8:Q8" si="24">QUOTIENT(D1+1,5)</f>
+        <v>0</v>
+      </c>
+      <c r="E8" s="13">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="F8" s="13">
+        <f t="shared" si="24"/>
+        <v>1</v>
+      </c>
+      <c r="G8" s="13">
+        <f t="shared" si="24"/>
+        <v>1</v>
+      </c>
+      <c r="H8" s="13">
+        <f t="shared" si="24"/>
+        <v>1</v>
+      </c>
+      <c r="I8" s="13">
+        <f t="shared" si="24"/>
+        <v>1</v>
+      </c>
+      <c r="J8" s="13">
+        <f t="shared" si="24"/>
+        <v>1</v>
+      </c>
+      <c r="K8" s="13">
+        <f t="shared" si="24"/>
+        <v>2</v>
+      </c>
+      <c r="L8" s="13">
+        <f t="shared" si="24"/>
+        <v>2</v>
+      </c>
+      <c r="M8" s="13">
+        <f t="shared" si="24"/>
+        <v>2</v>
+      </c>
+      <c r="N8" s="13">
+        <f t="shared" si="24"/>
+        <v>2</v>
+      </c>
+      <c r="O8" s="13">
+        <f t="shared" si="24"/>
+        <v>2</v>
+      </c>
+      <c r="P8" s="13">
+        <f t="shared" si="24"/>
+        <v>3</v>
+      </c>
+      <c r="Q8" s="42">
+        <f t="shared" si="24"/>
+        <v>3</v>
+      </c>
+      <c r="R8" s="42">
+        <f t="shared" ref="R8:V8" si="25">QUOTIENT(R1+1,5)</f>
+        <v>3</v>
+      </c>
+      <c r="S8" s="42">
+        <f t="shared" si="25"/>
+        <v>3</v>
+      </c>
+      <c r="T8" s="42">
+        <f t="shared" si="25"/>
+        <v>3</v>
+      </c>
+      <c r="U8" s="42">
+        <f t="shared" si="25"/>
+        <v>4</v>
+      </c>
+      <c r="V8" s="42">
+        <f t="shared" si="25"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A9" s="46" t="s">
+        <v>63</v>
+      </c>
+      <c r="B9" s="46" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="15">
+        <f>QUOTIENT(C1,6)</f>
+        <v>0</v>
+      </c>
+      <c r="D9" s="15">
+        <f t="shared" ref="D9:Q9" si="26">QUOTIENT(D1,6)</f>
+        <v>0</v>
+      </c>
+      <c r="E9" s="15">
+        <f t="shared" si="26"/>
+        <v>0</v>
+      </c>
+      <c r="F9" s="15">
+        <f t="shared" si="26"/>
+        <v>0</v>
+      </c>
+      <c r="G9" s="15">
+        <f t="shared" si="26"/>
+        <v>0</v>
+      </c>
+      <c r="H9" s="15">
+        <f t="shared" si="26"/>
+        <v>1</v>
+      </c>
+      <c r="I9" s="15">
+        <f t="shared" si="26"/>
+        <v>1</v>
+      </c>
+      <c r="J9" s="15">
+        <f t="shared" si="26"/>
+        <v>1</v>
+      </c>
+      <c r="K9" s="15">
+        <f t="shared" si="26"/>
+        <v>1</v>
+      </c>
+      <c r="L9" s="15">
+        <f t="shared" si="26"/>
+        <v>1</v>
+      </c>
+      <c r="M9" s="15">
+        <f t="shared" si="26"/>
+        <v>1</v>
+      </c>
+      <c r="N9" s="15">
+        <f t="shared" si="26"/>
+        <v>2</v>
+      </c>
+      <c r="O9" s="15">
+        <f t="shared" si="26"/>
+        <v>2</v>
+      </c>
+      <c r="P9" s="15">
+        <f t="shared" si="26"/>
+        <v>2</v>
+      </c>
+      <c r="Q9" s="43">
+        <f t="shared" si="26"/>
+        <v>2</v>
+      </c>
+      <c r="R9" s="43">
+        <f t="shared" ref="R9:V9" si="27">QUOTIENT(R1,6)</f>
+        <v>2</v>
+      </c>
+      <c r="S9" s="43">
+        <f t="shared" si="27"/>
+        <v>2</v>
+      </c>
+      <c r="T9" s="43">
+        <f t="shared" si="27"/>
+        <v>3</v>
+      </c>
+      <c r="U9" s="43">
+        <f t="shared" si="27"/>
+        <v>3</v>
+      </c>
+      <c r="V9" s="43">
+        <f t="shared" si="27"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B10" s="49" t="s">
+        <v>64</v>
+      </c>
+      <c r="C10" s="17">
+        <f>SUM(C2:C9)</f>
+        <v>3</v>
+      </c>
+      <c r="D10" s="56">
+        <f t="shared" ref="D10:Q10" si="28">SUM(D2:D9)</f>
+        <v>4</v>
+      </c>
+      <c r="E10" s="50">
+        <f t="shared" si="28"/>
+        <v>6</v>
+      </c>
+      <c r="F10" s="56">
+        <f t="shared" si="28"/>
+        <v>9</v>
+      </c>
+      <c r="G10" s="50">
+        <f t="shared" si="28"/>
+        <v>10</v>
+      </c>
+      <c r="H10" s="56">
+        <f t="shared" si="28"/>
+        <v>12</v>
+      </c>
+      <c r="I10" s="50">
+        <f t="shared" si="28"/>
+        <v>14</v>
+      </c>
+      <c r="J10" s="56">
+        <f t="shared" si="28"/>
+        <v>16</v>
+      </c>
+      <c r="K10" s="50">
+        <f t="shared" si="28"/>
+        <v>18</v>
+      </c>
+      <c r="L10" s="56">
+        <f t="shared" si="28"/>
+        <v>19</v>
+      </c>
+      <c r="M10" s="50">
+        <f t="shared" si="28"/>
+        <v>21</v>
+      </c>
+      <c r="N10" s="56">
+        <f t="shared" si="28"/>
+        <v>24</v>
+      </c>
+      <c r="O10" s="50">
+        <f t="shared" si="28"/>
+        <v>25</v>
+      </c>
+      <c r="P10" s="56">
+        <f t="shared" si="28"/>
+        <v>27</v>
+      </c>
+      <c r="Q10" s="56">
+        <f t="shared" si="28"/>
+        <v>29</v>
+      </c>
+      <c r="R10" s="56">
+        <f t="shared" ref="R10" si="29">SUM(R2:R9)</f>
+        <v>31</v>
+      </c>
+      <c r="S10" s="56">
+        <f t="shared" ref="S10" si="30">SUM(S2:S9)</f>
+        <v>32</v>
+      </c>
+      <c r="T10" s="56">
+        <f t="shared" ref="T10" si="31">SUM(T2:T9)</f>
+        <v>34</v>
+      </c>
+      <c r="U10" s="56">
+        <f t="shared" ref="U10" si="32">SUM(U2:U9)</f>
+        <v>37</v>
+      </c>
+      <c r="V10" s="56">
+        <f t="shared" ref="V10" si="33">SUM(V2:V9)</f>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B11" s="45" t="s">
+        <v>66</v>
+      </c>
+      <c r="C11" s="58">
+        <f>SUM(C5,(C6*3),(C7*9),C8,C9)</f>
+        <v>3</v>
+      </c>
+      <c r="D11" s="58">
+        <f t="shared" ref="D11:V11" si="34">SUM(D5,(D6*3),(D7*9),D8,D9)</f>
+        <v>4</v>
+      </c>
+      <c r="E11" s="58">
+        <f t="shared" si="34"/>
+        <v>3</v>
+      </c>
+      <c r="F11" s="58">
+        <f t="shared" si="34"/>
+        <v>18</v>
+      </c>
+      <c r="G11" s="58">
+        <f t="shared" si="34"/>
+        <v>16</v>
+      </c>
+      <c r="H11" s="58">
+        <f t="shared" si="34"/>
+        <v>20</v>
+      </c>
+      <c r="I11" s="58">
+        <f t="shared" si="34"/>
+        <v>20</v>
+      </c>
+      <c r="J11" s="58">
+        <f t="shared" si="34"/>
+        <v>32</v>
+      </c>
+      <c r="K11" s="58">
+        <f t="shared" si="34"/>
+        <v>30</v>
+      </c>
+      <c r="L11" s="58">
+        <f t="shared" si="34"/>
+        <v>37</v>
+      </c>
+      <c r="M11" s="58">
+        <f t="shared" si="34"/>
+        <v>33</v>
+      </c>
+      <c r="N11" s="58">
+        <f t="shared" si="34"/>
+        <v>48</v>
+      </c>
+      <c r="O11" s="58">
+        <f t="shared" si="34"/>
+        <v>46</v>
+      </c>
+      <c r="P11" s="58">
+        <f t="shared" si="34"/>
+        <v>52</v>
+      </c>
+      <c r="Q11" s="58">
+        <f t="shared" si="34"/>
+        <v>47</v>
+      </c>
+      <c r="R11" s="58">
+        <f t="shared" si="34"/>
+        <v>65</v>
+      </c>
+      <c r="S11" s="58">
+        <f t="shared" si="34"/>
+        <v>59</v>
+      </c>
+      <c r="T11" s="58">
+        <f t="shared" si="34"/>
+        <v>67</v>
+      </c>
+      <c r="U11" s="58">
+        <f t="shared" si="34"/>
+        <v>64</v>
+      </c>
+      <c r="V11" s="58">
+        <f t="shared" si="34"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B12" s="46" t="s">
+        <v>65</v>
+      </c>
+      <c r="C12" s="19">
+        <f>SUM(C2,(C3*3),(C4*9),C5,(C6*3),(C7*9),C8,C9)</f>
+        <v>7</v>
+      </c>
+      <c r="D12" s="57">
+        <f>SUM(D2,(D3*3),(D4*9),D5,(D6*3),(D7*9),D8,D9)</f>
+        <v>10</v>
+      </c>
+      <c r="E12" s="51">
+        <f>SUM(E2,(E3*3),(E4*9),E5,(E6*3),(E7*9),E8,E9)</f>
+        <v>20</v>
+      </c>
+      <c r="F12" s="57">
+        <f>SUM(F2,(F3*3),(F4*9),F5,(F6*3),(F7*9),F8,F9)</f>
+        <v>33</v>
+      </c>
+      <c r="G12" s="51">
+        <f>SUM(G2,(G3*3),(G4*9),G5,(G6*3),(G7*9),G8,G9)</f>
+        <v>36</v>
+      </c>
+      <c r="H12" s="57">
+        <f>SUM(H2,(H3*3),(H4*9),H5,(H6*3),(H7*9),H8,H9)</f>
+        <v>38</v>
+      </c>
+      <c r="I12" s="51">
+        <f>SUM(I2,(I3*3),(I4*9),I5,(I6*3),(I7*9),I8,I9)</f>
+        <v>50</v>
+      </c>
+      <c r="J12" s="57">
+        <f>SUM(J2,(J3*3),(J4*9),J5,(J6*3),(J7*9),J8,J9)</f>
+        <v>62</v>
+      </c>
+      <c r="K12" s="51">
+        <f>SUM(K2,(K3*3),(K4*9),K5,(K6*3),(K7*9),K8,K9)</f>
+        <v>64</v>
+      </c>
+      <c r="L12" s="57">
+        <f>SUM(L2,(L3*3),(L4*9),L5,(L6*3),(L7*9),L8,L9)</f>
+        <v>67</v>
+      </c>
+      <c r="M12" s="51">
+        <f>SUM(M2,(M3*3),(M4*9),M5,(M6*3),(M7*9),M8,M9)</f>
+        <v>79</v>
+      </c>
+      <c r="N12" s="57">
+        <f>SUM(N2,(N3*3),(N4*9),N5,(N6*3),(N7*9),N8,N9)</f>
+        <v>90</v>
+      </c>
+      <c r="O12" s="51">
+        <f>SUM(O2,(O3*3),(O4*9),O5,(O6*3),(O7*9),O8,O9)</f>
+        <v>93</v>
+      </c>
+      <c r="P12" s="57">
+        <f>SUM(P2,(P3*3),(P4*9),P5,(P6*3),(P7*9),P8,P9)</f>
+        <v>97</v>
+      </c>
+      <c r="Q12" s="57">
+        <f>SUM(Q2,(Q3*3),(Q4*9),Q5,(Q6*3),(Q7*9),Q8,Q9)</f>
+        <v>107</v>
+      </c>
+      <c r="R12" s="57">
+        <f>SUM(R2,(R3*3),(R4*9),R5,(R6*3),(R7*9),R8,R9)</f>
+        <v>119</v>
+      </c>
+      <c r="S12" s="57">
+        <f>SUM(S2,(S3*3),(S4*9),S5,(S6*3),(S7*9),S8,S9)</f>
+        <v>122</v>
+      </c>
+      <c r="T12" s="57">
+        <f>SUM(T2,(T3*3),(T4*9),T5,(T6*3),(T7*9),T8,T9)</f>
+        <v>124</v>
+      </c>
+      <c r="U12" s="57">
+        <f>SUM(U2,(U3*3),(U4*9),U5,(U6*3),(U7*9),U8,U9)</f>
+        <v>137</v>
+      </c>
+      <c r="V12" s="57">
+        <f>SUM(V2,(V3*3),(V4*9),V5,(V6*3),(V7*9),V8,V9)</f>
+        <v>149</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>